<commit_message>
Integration up to task 7
</commit_message>
<xml_diff>
--- a/Abgabe/Stations_BY.xlsx
+++ b/Abgabe/Stations_BY.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="356">
   <si>
     <t>Code</t>
   </si>
@@ -25,7 +25,7 @@
     <t>Location</t>
   </si>
   <si>
-    <t>x2</t>
+    <t>Code_Name</t>
   </si>
   <si>
     <t>Construction_Date</t>
@@ -58,7 +58,7 @@
     <t>Settings_Long</t>
   </si>
   <si>
-    <t>Seeings_Short</t>
+    <t>Settings_Short</t>
   </si>
   <si>
     <t>Type</t>
@@ -70,7 +70,7 @@
     <t>Street_Number</t>
   </si>
   <si>
-    <t>x6</t>
+    <t>ZIP_Code</t>
   </si>
   <si>
     <t>ID</t>
@@ -706,667 +706,211 @@
     <t>L 1.18</t>
   </si>
   <si>
-    <t>1989-07-01</t>
-  </si>
-  <si>
-    <t>1980-01-01</t>
-  </si>
-  <si>
-    <t>1978-08-01</t>
-  </si>
-  <si>
-    <t>1975-01-01</t>
-  </si>
-  <si>
-    <t>1986-08-01</t>
-  </si>
-  <si>
-    <t>1978-01-01</t>
-  </si>
-  <si>
-    <t>1976-01-01</t>
-  </si>
-  <si>
-    <t>1977-03-01</t>
-  </si>
-  <si>
-    <t>1987-02-01</t>
-  </si>
-  <si>
-    <t>1988-06-01</t>
-  </si>
-  <si>
-    <t>1989-06-01</t>
-  </si>
-  <si>
-    <t>2015-10-22</t>
-  </si>
-  <si>
-    <t>1988-10-01</t>
-  </si>
-  <si>
-    <t>1985-12-01</t>
-  </si>
-  <si>
-    <t>2013-12-12</t>
-  </si>
-  <si>
-    <t>1986-01-01</t>
-  </si>
-  <si>
-    <t>1986-09-01</t>
-  </si>
-  <si>
-    <t>1990-11-01</t>
-  </si>
-  <si>
-    <t>1989-02-01</t>
-  </si>
-  <si>
-    <t>2015-03-11</t>
-  </si>
-  <si>
-    <t>1983-10-01</t>
-  </si>
-  <si>
-    <t>2017-12-05</t>
-  </si>
-  <si>
-    <t>1992-05-01</t>
-  </si>
-  <si>
-    <t>1993-07-01</t>
-  </si>
-  <si>
-    <t>1999-05-11</t>
-  </si>
-  <si>
-    <t>2000-07-27</t>
-  </si>
-  <si>
-    <t>2003-04-17</t>
-  </si>
-  <si>
-    <t>2003-08-01</t>
-  </si>
-  <si>
-    <t>2004-04-01</t>
-  </si>
-  <si>
-    <t>2004-07-01</t>
-  </si>
-  <si>
-    <t>2005-04-05</t>
-  </si>
-  <si>
-    <t>2005-11-01</t>
-  </si>
-  <si>
-    <t>2006-11-01</t>
-  </si>
-  <si>
-    <t>2008-01-01</t>
-  </si>
-  <si>
-    <t>2010-06-21</t>
-  </si>
-  <si>
-    <t>2015-07-24</t>
-  </si>
-  <si>
-    <t>2012-07-26</t>
-  </si>
-  <si>
-    <t>2012-07-01</t>
-  </si>
-  <si>
-    <t>2014-01-28</t>
-  </si>
-  <si>
-    <t>2016-01-01</t>
-  </si>
-  <si>
-    <t>10.5723</t>
-  </si>
-  <si>
-    <t>12.1887</t>
-  </si>
-  <si>
-    <t>9.1715</t>
-  </si>
-  <si>
-    <t>9.1180</t>
-  </si>
-  <si>
-    <t>10.8950</t>
-  </si>
-  <si>
-    <t>10.8884</t>
-  </si>
-  <si>
-    <t>10.8877</t>
-  </si>
-  <si>
-    <t>12.8293</t>
-  </si>
-  <si>
-    <t>12.7814</t>
-  </si>
-  <si>
-    <t>10.9593</t>
-  </si>
-  <si>
-    <t>11.8975</t>
-  </si>
-  <si>
-    <t>11.4288</t>
-  </si>
-  <si>
-    <t>11.6383</t>
-  </si>
-  <si>
-    <t>11.8792</t>
-  </si>
-  <si>
-    <t>11.9488</t>
-  </si>
-  <si>
-    <t>10.3066</t>
-  </si>
-  <si>
-    <t>11.4426</t>
-  </si>
-  <si>
-    <t>12.1571</t>
-  </si>
-  <si>
-    <t>9.6889</t>
-  </si>
-  <si>
-    <t>11.5649</t>
-  </si>
-  <si>
-    <t>11.5547</t>
-  </si>
-  <si>
-    <t>11.7216</t>
-  </si>
-  <si>
-    <t>11.7778</t>
-  </si>
-  <si>
-    <t>10.0083</t>
-  </si>
-  <si>
-    <t>11.0884</t>
-  </si>
-  <si>
-    <t>10.9847</t>
-  </si>
-  <si>
-    <t>11.0248</t>
-  </si>
-  <si>
-    <t>13.1289</t>
-  </si>
-  <si>
-    <t>12.1016</t>
-  </si>
-  <si>
-    <t>12.1281</t>
-  </si>
-  <si>
-    <t>10.2321</t>
-  </si>
-  <si>
-    <t>12.5489</t>
-  </si>
-  <si>
-    <t>12.1594</t>
-  </si>
-  <si>
-    <t>9.9564</t>
-  </si>
-  <si>
-    <t>12.8912</t>
-  </si>
-  <si>
-    <t>12.5382</t>
-  </si>
-  <si>
-    <t>11.6480</t>
-  </si>
-  <si>
-    <t>11.7863</t>
-  </si>
-  <si>
-    <t>10.9031</t>
-  </si>
-  <si>
-    <t>11.2202</t>
-  </si>
-  <si>
-    <t>10.8962</t>
-  </si>
-  <si>
-    <t>11.5701</t>
-  </si>
-  <si>
-    <t>10.9635</t>
-  </si>
-  <si>
-    <t>11.5365</t>
-  </si>
-  <si>
-    <t>13.4220</t>
-  </si>
-  <si>
-    <t>9.9477</t>
-  </si>
-  <si>
-    <t>11.0361</t>
-  </si>
-  <si>
-    <t>12.1883</t>
-  </si>
-  <si>
-    <t>10.4042</t>
-  </si>
-  <si>
-    <t>10.3250</t>
-  </si>
-  <si>
-    <t>10.5977</t>
-  </si>
-  <si>
-    <t>11.0279</t>
-  </si>
-  <si>
-    <t>11.4645</t>
-  </si>
-  <si>
-    <t>11.0572</t>
-  </si>
-  <si>
-    <t>49.3049</t>
-  </si>
-  <si>
-    <t>50.0582</t>
-  </si>
-  <si>
-    <t>49.8694</t>
-  </si>
-  <si>
-    <t>49.9915</t>
-  </si>
-  <si>
-    <t>48.3646</t>
-  </si>
-  <si>
-    <t>48.3766</t>
-  </si>
-  <si>
-    <t>49.8983</t>
-  </si>
-  <si>
-    <t>48.1772</t>
-  </si>
-  <si>
-    <t>48.1828</t>
-  </si>
-  <si>
-    <t>50.2606</t>
-  </si>
-  <si>
-    <t>50.3206</t>
-  </si>
-  <si>
-    <t>48.7694</t>
-  </si>
-  <si>
-    <t>48.7671</t>
-  </si>
-  <si>
-    <t>48.9095</t>
-  </si>
-  <si>
-    <t>48.9042</t>
-  </si>
-  <si>
-    <t>47.7251</t>
-  </si>
-  <si>
-    <t>50.1031</t>
-  </si>
-  <si>
-    <t>48.5398</t>
-  </si>
-  <si>
-    <t>47.5575</t>
-  </si>
-  <si>
-    <t>48.1373</t>
-  </si>
-  <si>
-    <t>48.1545</t>
-  </si>
-  <si>
-    <t>50.3232</t>
-  </si>
-  <si>
-    <t>48.8532</t>
-  </si>
-  <si>
-    <t>48.3971</t>
-  </si>
-  <si>
-    <t>49.4459</t>
-  </si>
-  <si>
-    <t>49.4722</t>
-  </si>
-  <si>
-    <t>49.4622</t>
-  </si>
-  <si>
-    <t>48.9724</t>
-  </si>
-  <si>
-    <t>49.0152</t>
-  </si>
-  <si>
-    <t>49.3220</t>
-  </si>
-  <si>
-    <t>50.0484</t>
-  </si>
-  <si>
-    <t>49.4385</t>
-  </si>
-  <si>
-    <t>49.6790</t>
-  </si>
-  <si>
-    <t>49.8047</t>
-  </si>
-  <si>
-    <t>47.7334</t>
-  </si>
-  <si>
-    <t>48.0217</t>
-  </si>
-  <si>
-    <t>48.1732</t>
-  </si>
-  <si>
-    <t>49.4880</t>
-  </si>
-  <si>
-    <t>48.3260</t>
-  </si>
-  <si>
-    <t>47.9688</t>
-  </si>
-  <si>
-    <t>48.3702</t>
-  </si>
-  <si>
-    <t>49.9436</t>
-  </si>
-  <si>
-    <t>49.6059</t>
-  </si>
-  <si>
-    <t>48.1496</t>
-  </si>
-  <si>
-    <t>48.5736</t>
-  </si>
-  <si>
-    <t>49.7905</t>
-  </si>
-  <si>
-    <t>49.4405</t>
-  </si>
-  <si>
-    <t>47.6485</t>
-  </si>
-  <si>
-    <t>47.5180</t>
-  </si>
-  <si>
-    <t>49.4441</t>
-  </si>
-  <si>
-    <t>48.9522</t>
-  </si>
-  <si>
-    <t>49.3227</t>
-  </si>
-  <si>
-    <t>48.1817</t>
-  </si>
-  <si>
-    <t>47.4771</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>BY</t>
+  </si>
+  <si>
+    <t>Bavaria</t>
+  </si>
+  <si>
+    <t>urban area</t>
+  </si>
+  <si>
+    <t>suburban area</t>
+  </si>
+  <si>
+    <t>rural near town</t>
+  </si>
+  <si>
+    <t>rural regional</t>
+  </si>
+  <si>
+    <t>urban</t>
+  </si>
+  <si>
+    <t>suburban</t>
+  </si>
+  <si>
+    <t>rural</t>
+  </si>
+  <si>
+    <t>traffic</t>
+  </si>
+  <si>
+    <t>background</t>
+  </si>
+  <si>
+    <t>Residenzstraße/Brauhausstraße</t>
+  </si>
+  <si>
+    <t>Egerstraße</t>
+  </si>
+  <si>
+    <t>Hofstetter Straße</t>
+  </si>
+  <si>
+    <t>Bussardweg</t>
+  </si>
+  <si>
+    <t>Königsplatz</t>
+  </si>
+  <si>
+    <t>Bourges-Platz</t>
+  </si>
+  <si>
+    <t>Löwenbrücke</t>
+  </si>
+  <si>
+    <t>Klausenstraße</t>
+  </si>
+  <si>
+    <t>Scheibelbergstraße</t>
+  </si>
+  <si>
+    <t>Lossaustraße</t>
+  </si>
+  <si>
+    <t>Dr.-Enders-Straße</t>
+  </si>
+  <si>
+    <t>Rechbergstraße</t>
+  </si>
+  <si>
+    <t>Alter Wöhrer Weg</t>
+  </si>
+  <si>
+    <t>Regensburger Straße</t>
+  </si>
+  <si>
+    <t>Westend-/Bodmanstraße</t>
+  </si>
+  <si>
+    <t>Konrad-Adenauer-Straße</t>
+  </si>
+  <si>
+    <t>Podewilsstraße</t>
+  </si>
+  <si>
+    <t>Friedrichshafener Straße</t>
+  </si>
+  <si>
+    <t>Sonnenstraße</t>
+  </si>
+  <si>
+    <t>Lothstraße</t>
+  </si>
+  <si>
+    <t>Selbitzer Berg</t>
+  </si>
+  <si>
+    <t>KEH7 (Kreisstraße)</t>
+  </si>
+  <si>
+    <t>Gabelsberger-/Bahnhofstraße</t>
+  </si>
+  <si>
+    <t>Köhnstraße</t>
+  </si>
+  <si>
+    <t>Theresienstraße</t>
+  </si>
+  <si>
+    <t>Fuchsstraße</t>
+  </si>
+  <si>
+    <t>Bodenmaiser Straße</t>
+  </si>
+  <si>
+    <t>D.-Martin-Luther-Straße</t>
+  </si>
+  <si>
+    <t>Wackersdorfer Straße</t>
+  </si>
+  <si>
+    <t>Kornmarkt</t>
+  </si>
+  <si>
+    <t>Flurstück-Nr. 14</t>
+  </si>
+  <si>
+    <t>Nikolaistraße</t>
+  </si>
+  <si>
+    <t>Lindleinstraße</t>
+  </si>
+  <si>
+    <t>Kirchholzstraße</t>
+  </si>
+  <si>
+    <t>Schwimmbadstr.</t>
+  </si>
+  <si>
+    <t>Nußstraße</t>
+  </si>
+  <si>
+    <t>St.-Christophorus-Str.</t>
+  </si>
+  <si>
+    <t>Bürgermeister-Ulrich-Straße</t>
+  </si>
+  <si>
+    <t>Rothenfeld - JVA</t>
+  </si>
+  <si>
+    <t>Karlstraße</t>
+  </si>
+  <si>
+    <t>Hohenzollernring</t>
+  </si>
+  <si>
+    <t>Kraepelinstraße</t>
+  </si>
+  <si>
+    <t>Landshuter Allee</t>
+  </si>
+  <si>
+    <t>Stelzhamerstraße</t>
+  </si>
+  <si>
+    <t>Stadtring Süd</t>
+  </si>
+  <si>
+    <t>Von-der-Tann-Straße</t>
+  </si>
+  <si>
+    <t>Auenstraße</t>
+  </si>
+  <si>
+    <t>Riedlesweg</t>
+  </si>
+  <si>
+    <t>Grüne Au</t>
+  </si>
+  <si>
+    <t>Goethestraße</t>
+  </si>
+  <si>
+    <t>Angerstraße</t>
+  </si>
+  <si>
+    <t>Allacher Straße</t>
+  </si>
+  <si>
+    <t>Tegernauweg</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>ggüber 2</t>
+  </si>
+  <si>
+    <t>62</t>
   </si>
   <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>BY</t>
-  </si>
-  <si>
-    <t>Bavaria</t>
-  </si>
-  <si>
-    <t>urban area</t>
-  </si>
-  <si>
-    <t>suburban area</t>
-  </si>
-  <si>
-    <t>rural near town</t>
-  </si>
-  <si>
-    <t>rural regional</t>
-  </si>
-  <si>
-    <t>urban</t>
-  </si>
-  <si>
-    <t>suburban</t>
-  </si>
-  <si>
-    <t>rural</t>
-  </si>
-  <si>
-    <t>traffic</t>
-  </si>
-  <si>
-    <t>background</t>
-  </si>
-  <si>
-    <t>Residenzstraße/Brauhausstraße</t>
-  </si>
-  <si>
-    <t>Egerstraße</t>
-  </si>
-  <si>
-    <t>Hofstetter Straße</t>
-  </si>
-  <si>
-    <t>Bussardweg</t>
-  </si>
-  <si>
-    <t>Königsplatz</t>
-  </si>
-  <si>
-    <t>Bourges-Platz</t>
-  </si>
-  <si>
-    <t>Löwenbrücke</t>
-  </si>
-  <si>
-    <t>Klausenstraße</t>
-  </si>
-  <si>
-    <t>Scheibelbergstraße</t>
-  </si>
-  <si>
-    <t>Lossaustraße</t>
-  </si>
-  <si>
-    <t>Dr.-Enders-Straße</t>
-  </si>
-  <si>
-    <t>Rechbergstraße</t>
-  </si>
-  <si>
-    <t>Alter Wöhrer Weg</t>
-  </si>
-  <si>
-    <t>Regensburger Straße</t>
-  </si>
-  <si>
-    <t>Westend-/Bodmanstraße</t>
-  </si>
-  <si>
-    <t>Konrad-Adenauer-Straße</t>
-  </si>
-  <si>
-    <t>Podewilsstraße</t>
-  </si>
-  <si>
-    <t>Friedrichshafener Straße</t>
-  </si>
-  <si>
-    <t>Sonnenstraße</t>
-  </si>
-  <si>
-    <t>Lothstraße</t>
-  </si>
-  <si>
-    <t>Selbitzer Berg</t>
-  </si>
-  <si>
-    <t>KEH7 (Kreisstraße)</t>
-  </si>
-  <si>
-    <t>Gabelsberger-/Bahnhofstraße</t>
-  </si>
-  <si>
-    <t>Köhnstraße</t>
-  </si>
-  <si>
-    <t>Theresienstraße</t>
-  </si>
-  <si>
-    <t>Fuchsstraße</t>
-  </si>
-  <si>
-    <t>Bodenmaiser Straße</t>
-  </si>
-  <si>
-    <t>D.-Martin-Luther-Straße</t>
-  </si>
-  <si>
-    <t>Wackersdorfer Straße</t>
-  </si>
-  <si>
-    <t>Kornmarkt</t>
-  </si>
-  <si>
-    <t>Flurstück-Nr. 14</t>
-  </si>
-  <si>
-    <t>Nikolaistraße</t>
-  </si>
-  <si>
-    <t>Lindleinstraße</t>
-  </si>
-  <si>
-    <t>Kirchholzstraße</t>
-  </si>
-  <si>
-    <t>Schwimmbadstr.</t>
-  </si>
-  <si>
-    <t>Nußstraße</t>
-  </si>
-  <si>
-    <t>St.-Christophorus-Str.</t>
-  </si>
-  <si>
-    <t>Bürgermeister-Ulrich-Straße</t>
-  </si>
-  <si>
-    <t>Rothenfeld - JVA</t>
-  </si>
-  <si>
-    <t>Karlstraße</t>
-  </si>
-  <si>
-    <t>Hohenzollernring</t>
-  </si>
-  <si>
-    <t>Kraepelinstraße</t>
-  </si>
-  <si>
-    <t>Landshuter Allee</t>
-  </si>
-  <si>
-    <t>Stelzhamerstraße</t>
-  </si>
-  <si>
-    <t>Stadtring Süd</t>
-  </si>
-  <si>
-    <t>Von-der-Tann-Straße</t>
-  </si>
-  <si>
-    <t>Auenstraße</t>
-  </si>
-  <si>
-    <t>Riedlesweg</t>
-  </si>
-  <si>
-    <t>Grüne Au</t>
-  </si>
-  <si>
-    <t>Goethestraße</t>
-  </si>
-  <si>
-    <t>Angerstraße</t>
-  </si>
-  <si>
-    <t>Allacher Straße</t>
-  </si>
-  <si>
-    <t>Tegernauweg</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>ggüber 2</t>
-  </si>
-  <si>
-    <t>62</t>
   </si>
   <si>
     <t>160</t>
@@ -1544,6 +1088,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -1596,11 +1143,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1976,44 +1524,44 @@
       <c r="D2" t="s">
         <v>182</v>
       </c>
-      <c r="F2" t="s">
-        <v>230</v>
-      </c>
-      <c r="H2" t="s">
-        <v>270</v>
-      </c>
-      <c r="I2" t="s">
-        <v>324</v>
-      </c>
-      <c r="J2" t="s">
-        <v>378</v>
-      </c>
-      <c r="K2" t="s">
-        <v>379</v>
-      </c>
-      <c r="L2" t="s">
-        <v>382</v>
+      <c r="F2" s="2">
+        <v>32690</v>
+      </c>
+      <c r="H2">
+        <v>10.5723</v>
+      </c>
+      <c r="I2">
+        <v>49.3049</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
       </c>
       <c r="M2" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N2" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O2" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P2" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q2" t="s">
-        <v>392</v>
+        <v>239</v>
       </c>
       <c r="R2" t="s">
-        <v>394</v>
+        <v>241</v>
       </c>
       <c r="T2" t="s">
-        <v>456</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -2029,47 +1577,47 @@
       <c r="D3" t="s">
         <v>183</v>
       </c>
-      <c r="F3" t="s">
-        <v>231</v>
-      </c>
-      <c r="H3" t="s">
-        <v>271</v>
-      </c>
-      <c r="I3" t="s">
-        <v>325</v>
-      </c>
-      <c r="J3" t="s">
-        <v>378</v>
-      </c>
-      <c r="K3" t="s">
-        <v>378</v>
-      </c>
-      <c r="L3" t="s">
-        <v>379</v>
+      <c r="F3" s="2">
+        <v>29221</v>
+      </c>
+      <c r="H3">
+        <v>12.1887</v>
+      </c>
+      <c r="I3">
+        <v>50.0582</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N3" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O3" t="s">
-        <v>386</v>
+        <v>233</v>
       </c>
       <c r="P3" t="s">
-        <v>390</v>
+        <v>237</v>
       </c>
       <c r="Q3" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R3" t="s">
-        <v>395</v>
+        <v>242</v>
       </c>
       <c r="S3" t="s">
-        <v>447</v>
+        <v>294</v>
       </c>
       <c r="T3" t="s">
-        <v>457</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -2085,47 +1633,47 @@
       <c r="D4" t="s">
         <v>184</v>
       </c>
-      <c r="F4" t="s">
-        <v>232</v>
-      </c>
-      <c r="H4" t="s">
-        <v>272</v>
-      </c>
-      <c r="I4" t="s">
-        <v>326</v>
-      </c>
-      <c r="J4" t="s">
-        <v>378</v>
-      </c>
-      <c r="K4" t="s">
-        <v>380</v>
-      </c>
-      <c r="L4" t="s">
-        <v>379</v>
+      <c r="F4" s="2">
+        <v>28703</v>
+      </c>
+      <c r="H4">
+        <v>9.1715</v>
+      </c>
+      <c r="I4">
+        <v>49.8694</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>6</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N4" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O4" t="s">
-        <v>387</v>
+        <v>234</v>
       </c>
       <c r="P4" t="s">
-        <v>391</v>
+        <v>238</v>
       </c>
       <c r="Q4" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R4" t="s">
-        <v>396</v>
+        <v>243</v>
       </c>
       <c r="S4" t="s">
-        <v>448</v>
+        <v>295</v>
       </c>
       <c r="T4" t="s">
-        <v>458</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -2141,47 +1689,47 @@
       <c r="D5" t="s">
         <v>185</v>
       </c>
-      <c r="F5" t="s">
-        <v>232</v>
-      </c>
-      <c r="H5" t="s">
-        <v>273</v>
-      </c>
-      <c r="I5" t="s">
-        <v>327</v>
-      </c>
-      <c r="J5" t="s">
-        <v>378</v>
-      </c>
-      <c r="K5" t="s">
-        <v>378</v>
-      </c>
-      <c r="L5" t="s">
-        <v>379</v>
+      <c r="F5" s="2">
+        <v>28703</v>
+      </c>
+      <c r="H5">
+        <v>9.118</v>
+      </c>
+      <c r="I5">
+        <v>49.9915</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N5" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O5" t="s">
-        <v>386</v>
+        <v>233</v>
       </c>
       <c r="P5" t="s">
-        <v>390</v>
+        <v>237</v>
       </c>
       <c r="Q5" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R5" t="s">
-        <v>397</v>
+        <v>244</v>
       </c>
       <c r="S5" t="s">
-        <v>449</v>
+        <v>296</v>
       </c>
       <c r="T5" t="s">
-        <v>459</v>
+        <v>307</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -2197,44 +1745,44 @@
       <c r="D6" t="s">
         <v>186</v>
       </c>
-      <c r="F6" t="s">
-        <v>233</v>
-      </c>
-      <c r="H6" t="s">
-        <v>274</v>
-      </c>
-      <c r="I6" t="s">
-        <v>328</v>
-      </c>
-      <c r="J6" t="s">
-        <v>378</v>
-      </c>
-      <c r="K6" t="s">
-        <v>379</v>
-      </c>
-      <c r="L6" t="s">
-        <v>382</v>
+      <c r="F6" s="2">
+        <v>27395</v>
+      </c>
+      <c r="H6">
+        <v>10.895</v>
+      </c>
+      <c r="I6">
+        <v>48.3646</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
       </c>
       <c r="M6" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N6" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O6" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P6" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q6" t="s">
-        <v>392</v>
+        <v>239</v>
       </c>
       <c r="R6" t="s">
-        <v>398</v>
+        <v>245</v>
       </c>
       <c r="T6" t="s">
-        <v>460</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -2250,44 +1798,44 @@
       <c r="D7" t="s">
         <v>186</v>
       </c>
-      <c r="F7" t="s">
-        <v>234</v>
-      </c>
-      <c r="H7" t="s">
-        <v>275</v>
-      </c>
-      <c r="I7" t="s">
-        <v>329</v>
-      </c>
-      <c r="J7" t="s">
-        <v>378</v>
-      </c>
-      <c r="K7" t="s">
-        <v>379</v>
-      </c>
-      <c r="L7" t="s">
-        <v>379</v>
+      <c r="F7" s="2">
+        <v>31625</v>
+      </c>
+      <c r="H7">
+        <v>10.8884</v>
+      </c>
+      <c r="I7">
+        <v>48.3766</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
       </c>
       <c r="M7" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N7" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O7" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P7" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q7" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R7" t="s">
-        <v>399</v>
+        <v>246</v>
       </c>
       <c r="T7" t="s">
-        <v>461</v>
+        <v>309</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -2303,44 +1851,44 @@
       <c r="D8" t="s">
         <v>187</v>
       </c>
-      <c r="F8" t="s">
-        <v>235</v>
-      </c>
-      <c r="H8" t="s">
-        <v>276</v>
-      </c>
-      <c r="I8" t="s">
-        <v>330</v>
-      </c>
-      <c r="J8" t="s">
-        <v>378</v>
-      </c>
-      <c r="K8" t="s">
-        <v>379</v>
-      </c>
-      <c r="L8" t="s">
-        <v>379</v>
+      <c r="F8" s="2">
+        <v>28491</v>
+      </c>
+      <c r="H8">
+        <v>10.8877</v>
+      </c>
+      <c r="I8">
+        <v>49.8983</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
       </c>
       <c r="M8" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N8" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O8" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P8" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q8" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R8" t="s">
-        <v>400</v>
+        <v>247</v>
       </c>
       <c r="T8" t="s">
-        <v>462</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -2356,44 +1904,44 @@
       <c r="D9" t="s">
         <v>188</v>
       </c>
-      <c r="F9" t="s">
-        <v>236</v>
-      </c>
-      <c r="H9" t="s">
-        <v>277</v>
-      </c>
-      <c r="I9" t="s">
-        <v>331</v>
-      </c>
-      <c r="J9" t="s">
-        <v>378</v>
-      </c>
-      <c r="K9" t="s">
-        <v>378</v>
-      </c>
-      <c r="L9" t="s">
-        <v>379</v>
+      <c r="F9" s="2">
+        <v>27760</v>
+      </c>
+      <c r="H9">
+        <v>12.8293</v>
+      </c>
+      <c r="I9">
+        <v>48.1772</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N9" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O9" t="s">
-        <v>386</v>
+        <v>233</v>
       </c>
       <c r="P9" t="s">
-        <v>390</v>
+        <v>237</v>
       </c>
       <c r="Q9" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R9" t="s">
-        <v>401</v>
+        <v>248</v>
       </c>
       <c r="T9" t="s">
-        <v>463</v>
+        <v>311</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -2409,44 +1957,44 @@
       <c r="D10" t="s">
         <v>189</v>
       </c>
-      <c r="F10" t="s">
-        <v>237</v>
-      </c>
-      <c r="H10" t="s">
-        <v>278</v>
-      </c>
-      <c r="I10" t="s">
-        <v>332</v>
-      </c>
-      <c r="J10" t="s">
-        <v>378</v>
-      </c>
-      <c r="K10" t="s">
-        <v>381</v>
-      </c>
-      <c r="L10" t="s">
-        <v>379</v>
+      <c r="F10" s="2">
+        <v>28185</v>
+      </c>
+      <c r="H10">
+        <v>12.7814</v>
+      </c>
+      <c r="I10">
+        <v>48.1828</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N10" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O10" t="s">
-        <v>388</v>
+        <v>235</v>
       </c>
       <c r="P10" t="s">
-        <v>391</v>
+        <v>238</v>
       </c>
       <c r="Q10" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R10" t="s">
-        <v>402</v>
+        <v>249</v>
       </c>
       <c r="T10" t="s">
-        <v>464</v>
+        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -2462,44 +2010,44 @@
       <c r="D11" t="s">
         <v>190</v>
       </c>
-      <c r="F11" t="s">
-        <v>238</v>
-      </c>
-      <c r="H11" t="s">
-        <v>279</v>
-      </c>
-      <c r="I11" t="s">
-        <v>333</v>
-      </c>
-      <c r="J11" t="s">
-        <v>378</v>
-      </c>
-      <c r="K11" t="s">
-        <v>379</v>
-      </c>
-      <c r="L11" t="s">
-        <v>382</v>
+      <c r="F11" s="2">
+        <v>31809</v>
+      </c>
+      <c r="H11">
+        <v>10.9593</v>
+      </c>
+      <c r="I11">
+        <v>50.2606</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>3</v>
       </c>
       <c r="M11" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N11" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O11" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P11" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q11" t="s">
-        <v>392</v>
+        <v>239</v>
       </c>
       <c r="R11" t="s">
-        <v>403</v>
+        <v>250</v>
       </c>
       <c r="T11" t="s">
-        <v>465</v>
+        <v>313</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -2515,44 +2063,44 @@
       <c r="D12" t="s">
         <v>191</v>
       </c>
-      <c r="F12" t="s">
-        <v>239</v>
-      </c>
-      <c r="H12" t="s">
-        <v>280</v>
-      </c>
-      <c r="I12" t="s">
-        <v>334</v>
-      </c>
-      <c r="J12" t="s">
-        <v>378</v>
-      </c>
-      <c r="K12" t="s">
-        <v>378</v>
-      </c>
-      <c r="L12" t="s">
-        <v>379</v>
+      <c r="F12" s="2">
+        <v>32295</v>
+      </c>
+      <c r="H12">
+        <v>11.8975</v>
+      </c>
+      <c r="I12">
+        <v>50.3206</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
       </c>
       <c r="M12" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N12" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O12" t="s">
-        <v>386</v>
+        <v>233</v>
       </c>
       <c r="P12" t="s">
-        <v>390</v>
+        <v>237</v>
       </c>
       <c r="Q12" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R12" t="s">
-        <v>404</v>
+        <v>251</v>
       </c>
       <c r="T12" t="s">
-        <v>466</v>
+        <v>314</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -2568,44 +2116,44 @@
       <c r="D13" t="s">
         <v>192</v>
       </c>
-      <c r="F13" t="s">
-        <v>240</v>
-      </c>
-      <c r="H13" t="s">
-        <v>281</v>
-      </c>
-      <c r="I13" t="s">
-        <v>335</v>
-      </c>
-      <c r="J13" t="s">
-        <v>378</v>
-      </c>
-      <c r="K13" t="s">
-        <v>379</v>
-      </c>
-      <c r="L13" t="s">
-        <v>382</v>
+      <c r="F13" s="2">
+        <v>32660</v>
+      </c>
+      <c r="H13">
+        <v>11.4288</v>
+      </c>
+      <c r="I13">
+        <v>48.7694</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>3</v>
       </c>
       <c r="M13" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N13" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O13" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P13" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q13" t="s">
-        <v>392</v>
+        <v>239</v>
       </c>
       <c r="R13" t="s">
-        <v>405</v>
+        <v>252</v>
       </c>
       <c r="T13" t="s">
-        <v>467</v>
+        <v>315</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -2621,44 +2169,44 @@
       <c r="D14" t="s">
         <v>193</v>
       </c>
-      <c r="F14" t="s">
-        <v>241</v>
-      </c>
-      <c r="H14" t="s">
-        <v>282</v>
-      </c>
-      <c r="I14" t="s">
-        <v>336</v>
-      </c>
-      <c r="J14" t="s">
-        <v>378</v>
-      </c>
-      <c r="K14" t="s">
-        <v>378</v>
-      </c>
-      <c r="L14" t="s">
-        <v>379</v>
+      <c r="F14" s="2">
+        <v>42299</v>
+      </c>
+      <c r="H14">
+        <v>11.6383</v>
+      </c>
+      <c r="I14">
+        <v>48.7671</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
       </c>
       <c r="M14" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N14" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O14" t="s">
-        <v>386</v>
+        <v>233</v>
       </c>
       <c r="P14" t="s">
-        <v>390</v>
+        <v>237</v>
       </c>
       <c r="Q14" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R14" t="s">
-        <v>406</v>
+        <v>253</v>
       </c>
       <c r="T14" t="s">
-        <v>468</v>
+        <v>316</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -2674,44 +2222,44 @@
       <c r="D15" t="s">
         <v>194</v>
       </c>
-      <c r="F15" t="s">
-        <v>233</v>
-      </c>
-      <c r="H15" t="s">
-        <v>283</v>
-      </c>
-      <c r="I15" t="s">
-        <v>337</v>
-      </c>
-      <c r="J15" t="s">
-        <v>378</v>
-      </c>
-      <c r="K15" t="s">
-        <v>379</v>
-      </c>
-      <c r="L15" t="s">
-        <v>382</v>
+      <c r="F15" s="2">
+        <v>27395</v>
+      </c>
+      <c r="H15">
+        <v>11.8792</v>
+      </c>
+      <c r="I15">
+        <v>48.9095</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>3</v>
       </c>
       <c r="M15" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N15" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O15" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P15" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q15" t="s">
-        <v>392</v>
+        <v>239</v>
       </c>
       <c r="R15" t="s">
-        <v>407</v>
+        <v>254</v>
       </c>
       <c r="T15" t="s">
-        <v>469</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -2727,44 +2275,44 @@
       <c r="D16" t="s">
         <v>195</v>
       </c>
-      <c r="F16" t="s">
-        <v>232</v>
-      </c>
-      <c r="H16" t="s">
-        <v>284</v>
-      </c>
-      <c r="I16" t="s">
-        <v>338</v>
-      </c>
-      <c r="J16" t="s">
-        <v>378</v>
-      </c>
-      <c r="K16" t="s">
-        <v>378</v>
-      </c>
-      <c r="L16" t="s">
-        <v>379</v>
+      <c r="F16" s="2">
+        <v>28703</v>
+      </c>
+      <c r="H16">
+        <v>11.9488</v>
+      </c>
+      <c r="I16">
+        <v>48.9042</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
       </c>
       <c r="M16" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N16" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O16" t="s">
-        <v>386</v>
+        <v>233</v>
       </c>
       <c r="P16" t="s">
-        <v>390</v>
+        <v>237</v>
       </c>
       <c r="Q16" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R16" t="s">
-        <v>407</v>
+        <v>254</v>
       </c>
       <c r="T16" t="s">
-        <v>470</v>
+        <v>318</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -2780,44 +2328,44 @@
       <c r="D17" t="s">
         <v>196</v>
       </c>
-      <c r="F17" t="s">
-        <v>236</v>
-      </c>
-      <c r="H17" t="s">
-        <v>285</v>
-      </c>
-      <c r="I17" t="s">
-        <v>339</v>
-      </c>
-      <c r="J17" t="s">
-        <v>378</v>
-      </c>
-      <c r="K17" t="s">
-        <v>378</v>
-      </c>
-      <c r="L17" t="s">
-        <v>379</v>
+      <c r="F17" s="2">
+        <v>27760</v>
+      </c>
+      <c r="H17">
+        <v>10.3066</v>
+      </c>
+      <c r="I17">
+        <v>47.7251</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
       </c>
       <c r="M17" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N17" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O17" t="s">
-        <v>386</v>
+        <v>233</v>
       </c>
       <c r="P17" t="s">
-        <v>390</v>
+        <v>237</v>
       </c>
       <c r="Q17" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R17" t="s">
-        <v>408</v>
+        <v>255</v>
       </c>
       <c r="T17" t="s">
-        <v>471</v>
+        <v>319</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -2833,44 +2381,44 @@
       <c r="D18" t="s">
         <v>197</v>
       </c>
-      <c r="F18" t="s">
-        <v>242</v>
-      </c>
-      <c r="H18" t="s">
-        <v>286</v>
-      </c>
-      <c r="I18" t="s">
-        <v>340</v>
-      </c>
-      <c r="J18" t="s">
-        <v>378</v>
-      </c>
-      <c r="K18" t="s">
-        <v>379</v>
-      </c>
-      <c r="L18" t="s">
-        <v>379</v>
+      <c r="F18" s="2">
+        <v>32417</v>
+      </c>
+      <c r="H18">
+        <v>11.4426</v>
+      </c>
+      <c r="I18">
+        <v>50.1031</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
       </c>
       <c r="M18" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N18" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O18" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P18" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q18" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R18" t="s">
-        <v>409</v>
+        <v>256</v>
       </c>
       <c r="T18" t="s">
-        <v>472</v>
+        <v>320</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -2886,44 +2434,44 @@
       <c r="D19" t="s">
         <v>198</v>
       </c>
-      <c r="F19" t="s">
-        <v>243</v>
-      </c>
-      <c r="H19" t="s">
-        <v>287</v>
-      </c>
-      <c r="I19" t="s">
-        <v>341</v>
-      </c>
-      <c r="J19" t="s">
-        <v>378</v>
-      </c>
-      <c r="K19" t="s">
-        <v>379</v>
-      </c>
-      <c r="L19" t="s">
-        <v>382</v>
+      <c r="F19" s="2">
+        <v>31382</v>
+      </c>
+      <c r="H19">
+        <v>12.1571</v>
+      </c>
+      <c r="I19">
+        <v>48.5398</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>3</v>
       </c>
       <c r="M19" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N19" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O19" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P19" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q19" t="s">
-        <v>392</v>
+        <v>239</v>
       </c>
       <c r="R19" t="s">
-        <v>410</v>
+        <v>257</v>
       </c>
       <c r="T19" t="s">
-        <v>473</v>
+        <v>321</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -2939,44 +2487,44 @@
       <c r="D20" t="s">
         <v>199</v>
       </c>
-      <c r="F20" t="s">
-        <v>244</v>
-      </c>
-      <c r="H20" t="s">
-        <v>288</v>
-      </c>
-      <c r="I20" t="s">
-        <v>342</v>
-      </c>
-      <c r="J20" t="s">
-        <v>378</v>
-      </c>
-      <c r="K20" t="s">
-        <v>379</v>
-      </c>
-      <c r="L20" t="s">
-        <v>382</v>
+      <c r="F20" s="2">
+        <v>41620</v>
+      </c>
+      <c r="H20">
+        <v>9.6889</v>
+      </c>
+      <c r="I20">
+        <v>47.5575</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>3</v>
       </c>
       <c r="M20" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N20" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O20" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P20" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q20" t="s">
-        <v>392</v>
+        <v>239</v>
       </c>
       <c r="R20" t="s">
-        <v>411</v>
+        <v>258</v>
       </c>
       <c r="T20" t="s">
-        <v>474</v>
+        <v>322</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -2992,44 +2540,44 @@
       <c r="D21" t="s">
         <v>200</v>
       </c>
-      <c r="F21" t="s">
-        <v>235</v>
-      </c>
-      <c r="H21" t="s">
-        <v>289</v>
-      </c>
-      <c r="I21" t="s">
-        <v>343</v>
-      </c>
-      <c r="J21" t="s">
-        <v>378</v>
-      </c>
-      <c r="K21" t="s">
-        <v>379</v>
-      </c>
-      <c r="L21" t="s">
-        <v>382</v>
+      <c r="F21" s="2">
+        <v>28491</v>
+      </c>
+      <c r="H21">
+        <v>11.5649</v>
+      </c>
+      <c r="I21">
+        <v>48.1373</v>
+      </c>
+      <c r="J21">
+        <v>2</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>3</v>
       </c>
       <c r="M21" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N21" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O21" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P21" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q21" t="s">
-        <v>392</v>
+        <v>239</v>
       </c>
       <c r="R21" t="s">
-        <v>412</v>
+        <v>259</v>
       </c>
       <c r="T21" t="s">
-        <v>475</v>
+        <v>323</v>
       </c>
     </row>
     <row r="22" spans="1:20">
@@ -3045,47 +2593,47 @@
       <c r="D22" t="s">
         <v>200</v>
       </c>
-      <c r="F22" t="s">
-        <v>235</v>
-      </c>
-      <c r="H22" t="s">
-        <v>290</v>
-      </c>
-      <c r="I22" t="s">
-        <v>344</v>
-      </c>
-      <c r="J22" t="s">
-        <v>378</v>
-      </c>
-      <c r="K22" t="s">
-        <v>379</v>
-      </c>
-      <c r="L22" t="s">
-        <v>379</v>
+      <c r="F22" s="2">
+        <v>28491</v>
+      </c>
+      <c r="H22">
+        <v>11.5547</v>
+      </c>
+      <c r="I22">
+        <v>48.1545</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
       </c>
       <c r="M22" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N22" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O22" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P22" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q22" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R22" t="s">
-        <v>413</v>
+        <v>260</v>
       </c>
       <c r="S22" t="s">
-        <v>450</v>
+        <v>297</v>
       </c>
       <c r="T22" t="s">
-        <v>475</v>
+        <v>323</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -3101,44 +2649,44 @@
       <c r="D23" t="s">
         <v>201</v>
       </c>
-      <c r="F23" t="s">
-        <v>245</v>
-      </c>
-      <c r="H23" t="s">
-        <v>291</v>
-      </c>
-      <c r="I23" t="s">
-        <v>345</v>
-      </c>
-      <c r="J23" t="s">
-        <v>378</v>
-      </c>
-      <c r="K23" t="s">
-        <v>380</v>
-      </c>
-      <c r="L23" t="s">
-        <v>379</v>
+      <c r="F23" s="2">
+        <v>31413</v>
+      </c>
+      <c r="H23">
+        <v>11.7216</v>
+      </c>
+      <c r="I23">
+        <v>50.3232</v>
+      </c>
+      <c r="J23">
+        <v>2</v>
+      </c>
+      <c r="K23">
+        <v>6</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
       </c>
       <c r="M23" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N23" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O23" t="s">
-        <v>387</v>
+        <v>234</v>
       </c>
       <c r="P23" t="s">
-        <v>391</v>
+        <v>238</v>
       </c>
       <c r="Q23" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R23" t="s">
-        <v>414</v>
+        <v>261</v>
       </c>
       <c r="T23" t="s">
-        <v>476</v>
+        <v>324</v>
       </c>
     </row>
     <row r="24" spans="1:20">
@@ -3154,44 +2702,44 @@
       <c r="D24" t="s">
         <v>202</v>
       </c>
-      <c r="F24" t="s">
-        <v>237</v>
-      </c>
-      <c r="H24" t="s">
-        <v>292</v>
-      </c>
-      <c r="I24" t="s">
-        <v>346</v>
-      </c>
-      <c r="J24" t="s">
-        <v>378</v>
-      </c>
-      <c r="K24" t="s">
-        <v>381</v>
-      </c>
-      <c r="L24" t="s">
-        <v>379</v>
+      <c r="F24" s="2">
+        <v>28185</v>
+      </c>
+      <c r="H24">
+        <v>11.7778</v>
+      </c>
+      <c r="I24">
+        <v>48.8532</v>
+      </c>
+      <c r="J24">
+        <v>2</v>
+      </c>
+      <c r="K24">
+        <v>5</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
       </c>
       <c r="M24" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N24" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O24" t="s">
-        <v>388</v>
+        <v>235</v>
       </c>
       <c r="P24" t="s">
-        <v>391</v>
+        <v>238</v>
       </c>
       <c r="Q24" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R24" t="s">
-        <v>415</v>
+        <v>262</v>
       </c>
       <c r="T24" t="s">
-        <v>477</v>
+        <v>325</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -3207,44 +2755,44 @@
       <c r="D25" t="s">
         <v>203</v>
       </c>
-      <c r="F25" t="s">
-        <v>235</v>
-      </c>
-      <c r="H25" t="s">
-        <v>293</v>
-      </c>
-      <c r="I25" t="s">
-        <v>347</v>
-      </c>
-      <c r="J25" t="s">
-        <v>378</v>
-      </c>
-      <c r="K25" t="s">
-        <v>379</v>
-      </c>
-      <c r="L25" t="s">
-        <v>379</v>
+      <c r="F25" s="2">
+        <v>28491</v>
+      </c>
+      <c r="H25">
+        <v>10.0083</v>
+      </c>
+      <c r="I25">
+        <v>48.3971</v>
+      </c>
+      <c r="J25">
+        <v>2</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
       </c>
       <c r="M25" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N25" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O25" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P25" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q25" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R25" t="s">
-        <v>416</v>
+        <v>263</v>
       </c>
       <c r="T25" t="s">
-        <v>478</v>
+        <v>326</v>
       </c>
     </row>
     <row r="26" spans="1:20">
@@ -3260,44 +2808,44 @@
       <c r="D26" t="s">
         <v>204</v>
       </c>
-      <c r="F26" t="s">
-        <v>246</v>
-      </c>
-      <c r="H26" t="s">
-        <v>294</v>
-      </c>
-      <c r="I26" t="s">
-        <v>348</v>
-      </c>
-      <c r="J26" t="s">
-        <v>378</v>
-      </c>
-      <c r="K26" t="s">
-        <v>379</v>
-      </c>
-      <c r="L26" t="s">
-        <v>382</v>
+      <c r="F26" s="2">
+        <v>31656</v>
+      </c>
+      <c r="H26">
+        <v>11.0884</v>
+      </c>
+      <c r="I26">
+        <v>49.4459</v>
+      </c>
+      <c r="J26">
+        <v>2</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>3</v>
       </c>
       <c r="M26" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N26" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O26" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P26" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q26" t="s">
-        <v>392</v>
+        <v>239</v>
       </c>
       <c r="R26" t="s">
-        <v>417</v>
+        <v>264</v>
       </c>
       <c r="T26" t="s">
-        <v>479</v>
+        <v>327</v>
       </c>
     </row>
     <row r="27" spans="1:20">
@@ -3313,44 +2861,44 @@
       <c r="D27" t="s">
         <v>205</v>
       </c>
-      <c r="F27" t="s">
-        <v>247</v>
-      </c>
-      <c r="H27" t="s">
-        <v>295</v>
-      </c>
-      <c r="I27" t="s">
-        <v>349</v>
-      </c>
-      <c r="J27" t="s">
-        <v>378</v>
-      </c>
-      <c r="K27" t="s">
-        <v>379</v>
-      </c>
-      <c r="L27" t="s">
-        <v>382</v>
+      <c r="F27" s="2">
+        <v>33178</v>
+      </c>
+      <c r="H27">
+        <v>10.9847</v>
+      </c>
+      <c r="I27">
+        <v>49.4722</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>3</v>
       </c>
       <c r="M27" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N27" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O27" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P27" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q27" t="s">
-        <v>392</v>
+        <v>239</v>
       </c>
       <c r="R27" t="s">
-        <v>418</v>
+        <v>265</v>
       </c>
       <c r="T27" t="s">
-        <v>480</v>
+        <v>328</v>
       </c>
     </row>
     <row r="28" spans="1:20">
@@ -3366,47 +2914,47 @@
       <c r="D28" t="s">
         <v>206</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="2">
+        <v>28703</v>
+      </c>
+      <c r="H28">
+        <v>11.0248</v>
+      </c>
+      <c r="I28">
+        <v>49.4622</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28" t="s">
+        <v>230</v>
+      </c>
+      <c r="N28" t="s">
+        <v>231</v>
+      </c>
+      <c r="O28" t="s">
         <v>232</v>
       </c>
-      <c r="H28" t="s">
-        <v>296</v>
-      </c>
-      <c r="I28" t="s">
-        <v>350</v>
-      </c>
-      <c r="J28" t="s">
-        <v>378</v>
-      </c>
-      <c r="K28" t="s">
-        <v>379</v>
-      </c>
-      <c r="L28" t="s">
-        <v>379</v>
-      </c>
-      <c r="M28" t="s">
-        <v>383</v>
-      </c>
-      <c r="N28" t="s">
-        <v>384</v>
-      </c>
-      <c r="O28" t="s">
-        <v>385</v>
-      </c>
       <c r="P28" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q28" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R28" t="s">
-        <v>419</v>
+        <v>266</v>
       </c>
       <c r="S28" t="s">
-        <v>448</v>
+        <v>295</v>
       </c>
       <c r="T28" t="s">
-        <v>481</v>
+        <v>329</v>
       </c>
     </row>
     <row r="29" spans="1:20">
@@ -3422,44 +2970,44 @@
       <c r="D29" t="s">
         <v>207</v>
       </c>
-      <c r="F29" t="s">
-        <v>248</v>
-      </c>
-      <c r="H29" t="s">
-        <v>297</v>
-      </c>
-      <c r="I29" t="s">
-        <v>351</v>
-      </c>
-      <c r="J29" t="s">
-        <v>378</v>
-      </c>
-      <c r="K29" t="s">
-        <v>378</v>
-      </c>
-      <c r="L29" t="s">
-        <v>379</v>
+      <c r="F29" s="2">
+        <v>32540</v>
+      </c>
+      <c r="H29">
+        <v>13.1289</v>
+      </c>
+      <c r="I29">
+        <v>48.9724</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+      <c r="K29">
+        <v>2</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
       </c>
       <c r="M29" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N29" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O29" t="s">
-        <v>386</v>
+        <v>233</v>
       </c>
       <c r="P29" t="s">
-        <v>390</v>
+        <v>237</v>
       </c>
       <c r="Q29" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R29" t="s">
-        <v>420</v>
+        <v>267</v>
       </c>
       <c r="T29" t="s">
-        <v>482</v>
+        <v>330</v>
       </c>
     </row>
     <row r="30" spans="1:20">
@@ -3475,44 +3023,44 @@
       <c r="D30" t="s">
         <v>208</v>
       </c>
-      <c r="F30" t="s">
-        <v>249</v>
-      </c>
-      <c r="H30" t="s">
-        <v>298</v>
-      </c>
-      <c r="I30" t="s">
-        <v>352</v>
-      </c>
-      <c r="J30" t="s">
-        <v>378</v>
-      </c>
-      <c r="K30" t="s">
-        <v>379</v>
-      </c>
-      <c r="L30" t="s">
-        <v>382</v>
+      <c r="F30" s="2">
+        <v>42074</v>
+      </c>
+      <c r="H30">
+        <v>12.1016</v>
+      </c>
+      <c r="I30">
+        <v>49.0152</v>
+      </c>
+      <c r="J30">
+        <v>2</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>3</v>
       </c>
       <c r="M30" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N30" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O30" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P30" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q30" t="s">
-        <v>392</v>
+        <v>239</v>
       </c>
       <c r="R30" t="s">
-        <v>421</v>
+        <v>268</v>
       </c>
       <c r="T30" t="s">
-        <v>483</v>
+        <v>331</v>
       </c>
     </row>
     <row r="31" spans="1:20">
@@ -3528,44 +3076,44 @@
       <c r="D31" t="s">
         <v>209</v>
       </c>
-      <c r="F31" t="s">
-        <v>231</v>
-      </c>
-      <c r="H31" t="s">
-        <v>299</v>
-      </c>
-      <c r="I31" t="s">
-        <v>353</v>
-      </c>
-      <c r="J31" t="s">
-        <v>378</v>
-      </c>
-      <c r="K31" t="s">
-        <v>378</v>
-      </c>
-      <c r="L31" t="s">
-        <v>379</v>
+      <c r="F31" s="2">
+        <v>29221</v>
+      </c>
+      <c r="H31">
+        <v>12.1281</v>
+      </c>
+      <c r="I31">
+        <v>49.322</v>
+      </c>
+      <c r="J31">
+        <v>2</v>
+      </c>
+      <c r="K31">
+        <v>2</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
       </c>
       <c r="M31" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N31" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O31" t="s">
-        <v>386</v>
+        <v>233</v>
       </c>
       <c r="P31" t="s">
-        <v>390</v>
+        <v>237</v>
       </c>
       <c r="Q31" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R31" t="s">
-        <v>422</v>
+        <v>269</v>
       </c>
       <c r="T31" t="s">
-        <v>484</v>
+        <v>332</v>
       </c>
     </row>
     <row r="32" spans="1:20">
@@ -3581,44 +3129,44 @@
       <c r="D32" t="s">
         <v>210</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="2">
+        <v>27760</v>
+      </c>
+      <c r="H32">
+        <v>10.2321</v>
+      </c>
+      <c r="I32">
+        <v>50.0484</v>
+      </c>
+      <c r="J32">
+        <v>2</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32" t="s">
+        <v>230</v>
+      </c>
+      <c r="N32" t="s">
+        <v>231</v>
+      </c>
+      <c r="O32" t="s">
+        <v>232</v>
+      </c>
+      <c r="P32" t="s">
         <v>236</v>
       </c>
-      <c r="H32" t="s">
-        <v>300</v>
-      </c>
-      <c r="I32" t="s">
-        <v>354</v>
-      </c>
-      <c r="J32" t="s">
-        <v>378</v>
-      </c>
-      <c r="K32" t="s">
-        <v>379</v>
-      </c>
-      <c r="L32" t="s">
-        <v>379</v>
-      </c>
-      <c r="M32" t="s">
-        <v>383</v>
-      </c>
-      <c r="N32" t="s">
-        <v>384</v>
-      </c>
-      <c r="O32" t="s">
-        <v>385</v>
-      </c>
-      <c r="P32" t="s">
-        <v>389</v>
-      </c>
       <c r="Q32" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R32" t="s">
-        <v>423</v>
+        <v>270</v>
       </c>
       <c r="T32" t="s">
-        <v>485</v>
+        <v>333</v>
       </c>
     </row>
     <row r="33" spans="1:20">
@@ -3634,44 +3182,44 @@
       <c r="D33" t="s">
         <v>211</v>
       </c>
-      <c r="F33" t="s">
-        <v>250</v>
-      </c>
-      <c r="H33" t="s">
-        <v>301</v>
-      </c>
-      <c r="I33" t="s">
-        <v>355</v>
-      </c>
-      <c r="J33" t="s">
-        <v>378</v>
-      </c>
-      <c r="K33" t="s">
-        <v>381</v>
-      </c>
-      <c r="L33" t="s">
-        <v>379</v>
+      <c r="F33" s="2">
+        <v>30590</v>
+      </c>
+      <c r="H33">
+        <v>12.5489</v>
+      </c>
+      <c r="I33">
+        <v>49.4385</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+      <c r="K33">
+        <v>5</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
       </c>
       <c r="M33" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N33" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O33" t="s">
-        <v>388</v>
+        <v>235</v>
       </c>
       <c r="P33" t="s">
-        <v>391</v>
+        <v>238</v>
       </c>
       <c r="Q33" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R33" t="s">
-        <v>424</v>
+        <v>271</v>
       </c>
       <c r="T33" t="s">
-        <v>486</v>
+        <v>334</v>
       </c>
     </row>
     <row r="34" spans="1:20">
@@ -3687,44 +3235,44 @@
       <c r="D34" t="s">
         <v>212</v>
       </c>
-      <c r="F34" t="s">
-        <v>231</v>
-      </c>
-      <c r="H34" t="s">
-        <v>302</v>
-      </c>
-      <c r="I34" t="s">
-        <v>356</v>
-      </c>
-      <c r="J34" t="s">
-        <v>378</v>
-      </c>
-      <c r="K34" t="s">
-        <v>379</v>
-      </c>
-      <c r="L34" t="s">
-        <v>379</v>
+      <c r="F34" s="2">
+        <v>29221</v>
+      </c>
+      <c r="H34">
+        <v>12.1594</v>
+      </c>
+      <c r="I34">
+        <v>49.679</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
       </c>
       <c r="M34" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N34" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O34" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P34" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q34" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R34" t="s">
-        <v>425</v>
+        <v>272</v>
       </c>
       <c r="T34" t="s">
-        <v>487</v>
+        <v>335</v>
       </c>
     </row>
     <row r="35" spans="1:20">
@@ -3740,44 +3288,44 @@
       <c r="D35" t="s">
         <v>213</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="2">
+        <v>27395</v>
+      </c>
+      <c r="H35">
+        <v>9.9564</v>
+      </c>
+      <c r="I35">
+        <v>49.8047</v>
+      </c>
+      <c r="J35">
+        <v>2</v>
+      </c>
+      <c r="K35">
+        <v>2</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35" t="s">
+        <v>230</v>
+      </c>
+      <c r="N35" t="s">
+        <v>231</v>
+      </c>
+      <c r="O35" t="s">
         <v>233</v>
       </c>
-      <c r="H35" t="s">
-        <v>303</v>
-      </c>
-      <c r="I35" t="s">
-        <v>357</v>
-      </c>
-      <c r="J35" t="s">
-        <v>378</v>
-      </c>
-      <c r="K35" t="s">
-        <v>378</v>
-      </c>
-      <c r="L35" t="s">
-        <v>379</v>
-      </c>
-      <c r="M35" t="s">
-        <v>383</v>
-      </c>
-      <c r="N35" t="s">
-        <v>384</v>
-      </c>
-      <c r="O35" t="s">
-        <v>386</v>
-      </c>
       <c r="P35" t="s">
-        <v>390</v>
+        <v>237</v>
       </c>
       <c r="Q35" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R35" t="s">
-        <v>426</v>
+        <v>273</v>
       </c>
       <c r="T35" t="s">
-        <v>488</v>
+        <v>336</v>
       </c>
     </row>
     <row r="36" spans="1:20">
@@ -3793,44 +3341,44 @@
       <c r="D36" t="s">
         <v>214</v>
       </c>
-      <c r="F36" t="s">
-        <v>251</v>
-      </c>
-      <c r="H36" t="s">
-        <v>304</v>
-      </c>
-      <c r="I36" t="s">
-        <v>358</v>
-      </c>
-      <c r="J36" t="s">
-        <v>378</v>
-      </c>
-      <c r="K36" t="s">
-        <v>379</v>
-      </c>
-      <c r="L36" t="s">
-        <v>379</v>
+      <c r="F36" s="2">
+        <v>43074</v>
+      </c>
+      <c r="H36">
+        <v>12.8912</v>
+      </c>
+      <c r="I36">
+        <v>47.7334</v>
+      </c>
+      <c r="J36">
+        <v>2</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
       </c>
       <c r="M36" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N36" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O36" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P36" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q36" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R36" t="s">
-        <v>427</v>
+        <v>274</v>
       </c>
       <c r="T36" t="s">
-        <v>489</v>
+        <v>337</v>
       </c>
     </row>
     <row r="37" spans="1:20">
@@ -3846,44 +3394,44 @@
       <c r="D37" t="s">
         <v>215</v>
       </c>
-      <c r="F37" t="s">
-        <v>252</v>
-      </c>
-      <c r="H37" t="s">
-        <v>305</v>
-      </c>
-      <c r="I37" t="s">
-        <v>359</v>
-      </c>
-      <c r="J37" t="s">
-        <v>378</v>
-      </c>
-      <c r="K37" t="s">
-        <v>378</v>
-      </c>
-      <c r="L37" t="s">
-        <v>379</v>
+      <c r="F37" s="2">
+        <v>33725</v>
+      </c>
+      <c r="H37">
+        <v>12.5382</v>
+      </c>
+      <c r="I37">
+        <v>48.0217</v>
+      </c>
+      <c r="J37">
+        <v>2</v>
+      </c>
+      <c r="K37">
+        <v>2</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
       </c>
       <c r="M37" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N37" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O37" t="s">
-        <v>386</v>
+        <v>233</v>
       </c>
       <c r="P37" t="s">
-        <v>390</v>
+        <v>237</v>
       </c>
       <c r="Q37" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R37" t="s">
-        <v>428</v>
+        <v>275</v>
       </c>
       <c r="T37" t="s">
-        <v>490</v>
+        <v>338</v>
       </c>
     </row>
     <row r="38" spans="1:20">
@@ -3899,44 +3447,44 @@
       <c r="D38" t="s">
         <v>216</v>
       </c>
-      <c r="F38" t="s">
-        <v>253</v>
-      </c>
-      <c r="H38" t="s">
-        <v>306</v>
-      </c>
-      <c r="I38" t="s">
-        <v>360</v>
-      </c>
-      <c r="J38" t="s">
-        <v>378</v>
-      </c>
-      <c r="K38" t="s">
-        <v>378</v>
-      </c>
-      <c r="L38" t="s">
-        <v>379</v>
+      <c r="F38" s="2">
+        <v>34151</v>
+      </c>
+      <c r="H38">
+        <v>11.648</v>
+      </c>
+      <c r="I38">
+        <v>48.1732</v>
+      </c>
+      <c r="J38">
+        <v>2</v>
+      </c>
+      <c r="K38">
+        <v>2</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
       </c>
       <c r="M38" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N38" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O38" t="s">
-        <v>386</v>
+        <v>233</v>
       </c>
       <c r="P38" t="s">
-        <v>390</v>
+        <v>237</v>
       </c>
       <c r="Q38" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R38" t="s">
-        <v>429</v>
+        <v>276</v>
       </c>
       <c r="T38" t="s">
-        <v>491</v>
+        <v>339</v>
       </c>
     </row>
     <row r="39" spans="1:20">
@@ -3952,47 +3500,47 @@
       <c r="D39" t="s">
         <v>217</v>
       </c>
-      <c r="F39" t="s">
-        <v>254</v>
-      </c>
-      <c r="H39" t="s">
-        <v>307</v>
-      </c>
-      <c r="I39" t="s">
-        <v>361</v>
-      </c>
-      <c r="J39" t="s">
-        <v>378</v>
-      </c>
-      <c r="K39" t="s">
-        <v>378</v>
-      </c>
-      <c r="L39" t="s">
-        <v>379</v>
+      <c r="F39" s="2">
+        <v>36291</v>
+      </c>
+      <c r="H39">
+        <v>11.7863</v>
+      </c>
+      <c r="I39">
+        <v>49.488</v>
+      </c>
+      <c r="J39">
+        <v>2</v>
+      </c>
+      <c r="K39">
+        <v>2</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
       </c>
       <c r="M39" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N39" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O39" t="s">
-        <v>386</v>
+        <v>233</v>
       </c>
       <c r="P39" t="s">
-        <v>390</v>
+        <v>237</v>
       </c>
       <c r="Q39" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R39" t="s">
-        <v>430</v>
+        <v>277</v>
       </c>
       <c r="S39" t="s">
-        <v>379</v>
+        <v>298</v>
       </c>
       <c r="T39" t="s">
-        <v>492</v>
+        <v>340</v>
       </c>
     </row>
     <row r="40" spans="1:20">
@@ -4008,47 +3556,47 @@
       <c r="D40" t="s">
         <v>186</v>
       </c>
-      <c r="F40" t="s">
-        <v>255</v>
-      </c>
-      <c r="H40" t="s">
-        <v>308</v>
-      </c>
-      <c r="I40" t="s">
-        <v>362</v>
-      </c>
-      <c r="J40" t="s">
-        <v>378</v>
-      </c>
-      <c r="K40" t="s">
-        <v>378</v>
-      </c>
-      <c r="L40" t="s">
-        <v>379</v>
+      <c r="F40" s="2">
+        <v>36734</v>
+      </c>
+      <c r="H40">
+        <v>10.9031</v>
+      </c>
+      <c r="I40">
+        <v>48.326</v>
+      </c>
+      <c r="J40">
+        <v>2</v>
+      </c>
+      <c r="K40">
+        <v>2</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
       </c>
       <c r="M40" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N40" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O40" t="s">
-        <v>386</v>
+        <v>233</v>
       </c>
       <c r="P40" t="s">
-        <v>390</v>
+        <v>237</v>
       </c>
       <c r="Q40" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R40" t="s">
-        <v>431</v>
+        <v>278</v>
       </c>
       <c r="S40" t="s">
-        <v>451</v>
+        <v>299</v>
       </c>
       <c r="T40" t="s">
-        <v>493</v>
+        <v>341</v>
       </c>
     </row>
     <row r="41" spans="1:20">
@@ -4064,44 +3612,44 @@
       <c r="D41" t="s">
         <v>218</v>
       </c>
-      <c r="F41" t="s">
-        <v>256</v>
-      </c>
-      <c r="H41" t="s">
-        <v>309</v>
-      </c>
-      <c r="I41" t="s">
-        <v>363</v>
-      </c>
-      <c r="J41" t="s">
-        <v>378</v>
-      </c>
-      <c r="K41" t="s">
-        <v>381</v>
-      </c>
-      <c r="L41" t="s">
-        <v>379</v>
+      <c r="F41" s="2">
+        <v>37728</v>
+      </c>
+      <c r="H41">
+        <v>11.2202</v>
+      </c>
+      <c r="I41">
+        <v>47.9688</v>
+      </c>
+      <c r="J41">
+        <v>2</v>
+      </c>
+      <c r="K41">
+        <v>5</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
       </c>
       <c r="M41" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N41" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O41" t="s">
-        <v>388</v>
+        <v>235</v>
       </c>
       <c r="P41" t="s">
-        <v>391</v>
+        <v>238</v>
       </c>
       <c r="Q41" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R41" t="s">
-        <v>432</v>
+        <v>279</v>
       </c>
       <c r="T41" t="s">
-        <v>494</v>
+        <v>342</v>
       </c>
     </row>
     <row r="42" spans="1:20">
@@ -4117,44 +3665,44 @@
       <c r="D42" t="s">
         <v>186</v>
       </c>
-      <c r="F42" t="s">
-        <v>257</v>
-      </c>
-      <c r="H42" t="s">
-        <v>310</v>
-      </c>
-      <c r="I42" t="s">
-        <v>364</v>
-      </c>
-      <c r="J42" t="s">
-        <v>378</v>
-      </c>
-      <c r="K42" t="s">
-        <v>379</v>
-      </c>
-      <c r="L42" t="s">
-        <v>382</v>
+      <c r="F42" s="2">
+        <v>37834</v>
+      </c>
+      <c r="H42">
+        <v>10.8962</v>
+      </c>
+      <c r="I42">
+        <v>48.3702</v>
+      </c>
+      <c r="J42">
+        <v>2</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <v>3</v>
       </c>
       <c r="M42" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N42" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O42" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P42" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q42" t="s">
-        <v>392</v>
+        <v>239</v>
       </c>
       <c r="R42" t="s">
-        <v>433</v>
+        <v>280</v>
       </c>
       <c r="T42" t="s">
-        <v>460</v>
+        <v>308</v>
       </c>
     </row>
     <row r="43" spans="1:20">
@@ -4170,44 +3718,44 @@
       <c r="D43" t="s">
         <v>219</v>
       </c>
-      <c r="F43" t="s">
-        <v>257</v>
-      </c>
-      <c r="H43" t="s">
-        <v>311</v>
-      </c>
-      <c r="I43" t="s">
-        <v>365</v>
-      </c>
-      <c r="J43" t="s">
-        <v>378</v>
-      </c>
-      <c r="K43" t="s">
-        <v>379</v>
-      </c>
-      <c r="L43" t="s">
-        <v>382</v>
+      <c r="F43" s="2">
+        <v>37834</v>
+      </c>
+      <c r="H43">
+        <v>11.5701</v>
+      </c>
+      <c r="I43">
+        <v>49.9436</v>
+      </c>
+      <c r="J43">
+        <v>2</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+      <c r="L43">
+        <v>3</v>
       </c>
       <c r="M43" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N43" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O43" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P43" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q43" t="s">
-        <v>392</v>
+        <v>239</v>
       </c>
       <c r="R43" t="s">
-        <v>434</v>
+        <v>281</v>
       </c>
       <c r="T43" t="s">
-        <v>495</v>
+        <v>343</v>
       </c>
     </row>
     <row r="44" spans="1:20">
@@ -4223,44 +3771,44 @@
       <c r="D44" t="s">
         <v>220</v>
       </c>
-      <c r="F44" t="s">
-        <v>258</v>
-      </c>
-      <c r="H44" t="s">
-        <v>312</v>
-      </c>
-      <c r="I44" t="s">
-        <v>366</v>
-      </c>
-      <c r="J44" t="s">
-        <v>378</v>
-      </c>
-      <c r="K44" t="s">
-        <v>378</v>
-      </c>
-      <c r="L44" t="s">
-        <v>379</v>
+      <c r="F44" s="2">
+        <v>38078</v>
+      </c>
+      <c r="H44">
+        <v>10.9635</v>
+      </c>
+      <c r="I44">
+        <v>49.6059</v>
+      </c>
+      <c r="J44">
+        <v>2</v>
+      </c>
+      <c r="K44">
+        <v>2</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
       </c>
       <c r="M44" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N44" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O44" t="s">
-        <v>386</v>
+        <v>233</v>
       </c>
       <c r="P44" t="s">
-        <v>390</v>
+        <v>237</v>
       </c>
       <c r="Q44" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R44" t="s">
-        <v>435</v>
+        <v>282</v>
       </c>
       <c r="T44" t="s">
-        <v>496</v>
+        <v>344</v>
       </c>
     </row>
     <row r="45" spans="1:20">
@@ -4276,47 +3824,47 @@
       <c r="D45" t="s">
         <v>200</v>
       </c>
-      <c r="F45" t="s">
-        <v>259</v>
-      </c>
-      <c r="H45" t="s">
-        <v>313</v>
-      </c>
-      <c r="I45" t="s">
-        <v>367</v>
-      </c>
-      <c r="J45" t="s">
-        <v>378</v>
-      </c>
-      <c r="K45" t="s">
-        <v>379</v>
-      </c>
-      <c r="L45" t="s">
-        <v>382</v>
+      <c r="F45" s="2">
+        <v>38169</v>
+      </c>
+      <c r="H45">
+        <v>11.5365</v>
+      </c>
+      <c r="I45">
+        <v>48.1496</v>
+      </c>
+      <c r="J45">
+        <v>2</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="L45">
+        <v>3</v>
       </c>
       <c r="M45" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N45" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O45" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P45" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q45" t="s">
-        <v>392</v>
+        <v>239</v>
       </c>
       <c r="R45" t="s">
-        <v>436</v>
+        <v>283</v>
       </c>
       <c r="S45" t="s">
-        <v>452</v>
+        <v>300</v>
       </c>
       <c r="T45" t="s">
-        <v>497</v>
+        <v>345</v>
       </c>
     </row>
     <row r="46" spans="1:20">
@@ -4332,44 +3880,44 @@
       <c r="D46" t="s">
         <v>221</v>
       </c>
-      <c r="F46" t="s">
-        <v>260</v>
-      </c>
-      <c r="H46" t="s">
-        <v>314</v>
-      </c>
-      <c r="I46" t="s">
-        <v>368</v>
-      </c>
-      <c r="J46" t="s">
-        <v>378</v>
-      </c>
-      <c r="K46" t="s">
-        <v>379</v>
-      </c>
-      <c r="L46" t="s">
-        <v>379</v>
+      <c r="F46" s="2">
+        <v>38447</v>
+      </c>
+      <c r="H46">
+        <v>13.422</v>
+      </c>
+      <c r="I46">
+        <v>48.5736</v>
+      </c>
+      <c r="J46">
+        <v>2</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
       </c>
       <c r="M46" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N46" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O46" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P46" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q46" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R46" t="s">
-        <v>437</v>
+        <v>284</v>
       </c>
       <c r="T46" t="s">
-        <v>498</v>
+        <v>346</v>
       </c>
     </row>
     <row r="47" spans="1:20">
@@ -4385,47 +3933,47 @@
       <c r="D47" t="s">
         <v>213</v>
       </c>
-      <c r="F47" t="s">
-        <v>261</v>
-      </c>
-      <c r="H47" t="s">
-        <v>315</v>
-      </c>
-      <c r="I47" t="s">
-        <v>369</v>
-      </c>
-      <c r="J47" t="s">
-        <v>378</v>
-      </c>
-      <c r="K47" t="s">
-        <v>379</v>
-      </c>
-      <c r="L47" t="s">
-        <v>382</v>
+      <c r="F47" s="2">
+        <v>38657</v>
+      </c>
+      <c r="H47">
+        <v>9.947699999999999</v>
+      </c>
+      <c r="I47">
+        <v>49.7905</v>
+      </c>
+      <c r="J47">
+        <v>2</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="L47">
+        <v>3</v>
       </c>
       <c r="M47" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N47" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O47" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P47" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q47" t="s">
-        <v>392</v>
+        <v>239</v>
       </c>
       <c r="R47" t="s">
-        <v>438</v>
+        <v>285</v>
       </c>
       <c r="S47" t="s">
-        <v>453</v>
+        <v>301</v>
       </c>
       <c r="T47" t="s">
-        <v>499</v>
+        <v>347</v>
       </c>
     </row>
     <row r="48" spans="1:20">
@@ -4441,47 +3989,47 @@
       <c r="D48" t="s">
         <v>204</v>
       </c>
-      <c r="F48" t="s">
-        <v>262</v>
-      </c>
-      <c r="H48" t="s">
-        <v>316</v>
-      </c>
-      <c r="I48" t="s">
-        <v>370</v>
-      </c>
-      <c r="J48" t="s">
-        <v>378</v>
-      </c>
-      <c r="K48" t="s">
-        <v>379</v>
-      </c>
-      <c r="L48" t="s">
-        <v>382</v>
+      <c r="F48" s="2">
+        <v>39022</v>
+      </c>
+      <c r="H48">
+        <v>11.0361</v>
+      </c>
+      <c r="I48">
+        <v>49.4405</v>
+      </c>
+      <c r="J48">
+        <v>2</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <v>3</v>
       </c>
       <c r="M48" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N48" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O48" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P48" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q48" t="s">
-        <v>392</v>
+        <v>239</v>
       </c>
       <c r="R48" t="s">
-        <v>439</v>
+        <v>286</v>
       </c>
       <c r="S48" t="s">
-        <v>454</v>
+        <v>302</v>
       </c>
       <c r="T48" t="s">
-        <v>500</v>
+        <v>348</v>
       </c>
     </row>
     <row r="49" spans="1:20">
@@ -4497,44 +4045,44 @@
       <c r="D49" t="s">
         <v>222</v>
       </c>
-      <c r="F49" t="s">
-        <v>263</v>
-      </c>
-      <c r="H49" t="s">
-        <v>317</v>
-      </c>
-      <c r="I49" t="s">
-        <v>371</v>
-      </c>
-      <c r="J49" t="s">
-        <v>378</v>
-      </c>
-      <c r="K49" t="s">
-        <v>380</v>
-      </c>
-      <c r="L49" t="s">
-        <v>382</v>
+      <c r="F49" s="2">
+        <v>39448</v>
+      </c>
+      <c r="H49">
+        <v>12.1883</v>
+      </c>
+      <c r="I49">
+        <v>47.6485</v>
+      </c>
+      <c r="J49">
+        <v>2</v>
+      </c>
+      <c r="K49">
+        <v>6</v>
+      </c>
+      <c r="L49">
+        <v>3</v>
       </c>
       <c r="M49" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N49" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O49" t="s">
-        <v>387</v>
+        <v>234</v>
       </c>
       <c r="P49" t="s">
-        <v>391</v>
+        <v>238</v>
       </c>
       <c r="Q49" t="s">
-        <v>392</v>
+        <v>239</v>
       </c>
       <c r="R49" t="s">
-        <v>440</v>
+        <v>287</v>
       </c>
       <c r="T49" t="s">
-        <v>501</v>
+        <v>349</v>
       </c>
     </row>
     <row r="50" spans="1:20">
@@ -4550,44 +4098,44 @@
       <c r="D50" t="s">
         <v>223</v>
       </c>
-      <c r="F50" t="s">
-        <v>264</v>
-      </c>
-      <c r="H50" t="s">
-        <v>318</v>
-      </c>
-      <c r="I50" t="s">
-        <v>372</v>
-      </c>
-      <c r="J50" t="s">
-        <v>378</v>
-      </c>
-      <c r="K50" t="s">
-        <v>381</v>
-      </c>
-      <c r="L50" t="s">
-        <v>379</v>
+      <c r="F50" s="2">
+        <v>40350</v>
+      </c>
+      <c r="H50">
+        <v>10.4042</v>
+      </c>
+      <c r="I50">
+        <v>47.518</v>
+      </c>
+      <c r="J50">
+        <v>2</v>
+      </c>
+      <c r="K50">
+        <v>5</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
       </c>
       <c r="M50" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N50" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O50" t="s">
-        <v>388</v>
+        <v>235</v>
       </c>
       <c r="P50" t="s">
-        <v>391</v>
+        <v>238</v>
       </c>
       <c r="Q50" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R50" t="s">
-        <v>441</v>
+        <v>288</v>
       </c>
       <c r="T50" t="s">
-        <v>502</v>
+        <v>350</v>
       </c>
     </row>
     <row r="51" spans="1:20">
@@ -4603,44 +4151,44 @@
       <c r="D51" t="s">
         <v>224</v>
       </c>
-      <c r="F51" t="s">
-        <v>265</v>
-      </c>
-      <c r="H51" t="s">
-        <v>319</v>
-      </c>
-      <c r="I51" t="s">
-        <v>373</v>
-      </c>
-      <c r="J51" t="s">
-        <v>378</v>
-      </c>
-      <c r="K51" t="s">
-        <v>381</v>
-      </c>
-      <c r="L51" t="s">
-        <v>379</v>
+      <c r="F51" s="2">
+        <v>42209</v>
+      </c>
+      <c r="H51">
+        <v>10.325</v>
+      </c>
+      <c r="I51">
+        <v>49.4441</v>
+      </c>
+      <c r="J51">
+        <v>2</v>
+      </c>
+      <c r="K51">
+        <v>5</v>
+      </c>
+      <c r="L51">
+        <v>1</v>
       </c>
       <c r="M51" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N51" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O51" t="s">
-        <v>388</v>
+        <v>235</v>
       </c>
       <c r="P51" t="s">
-        <v>391</v>
+        <v>238</v>
       </c>
       <c r="Q51" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R51" t="s">
-        <v>442</v>
+        <v>289</v>
       </c>
       <c r="T51" t="s">
-        <v>503</v>
+        <v>351</v>
       </c>
     </row>
     <row r="52" spans="1:20">
@@ -4656,44 +4204,44 @@
       <c r="D52" t="s">
         <v>225</v>
       </c>
-      <c r="F52" t="s">
-        <v>266</v>
-      </c>
-      <c r="H52" t="s">
-        <v>320</v>
-      </c>
-      <c r="I52" t="s">
-        <v>374</v>
-      </c>
-      <c r="J52" t="s">
-        <v>378</v>
-      </c>
-      <c r="K52" t="s">
-        <v>378</v>
-      </c>
-      <c r="L52" t="s">
-        <v>379</v>
+      <c r="F52" s="2">
+        <v>41116</v>
+      </c>
+      <c r="H52">
+        <v>10.5977</v>
+      </c>
+      <c r="I52">
+        <v>48.9522</v>
+      </c>
+      <c r="J52">
+        <v>2</v>
+      </c>
+      <c r="K52">
+        <v>2</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
       </c>
       <c r="M52" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N52" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O52" t="s">
-        <v>386</v>
+        <v>233</v>
       </c>
       <c r="P52" t="s">
-        <v>390</v>
+        <v>237</v>
       </c>
       <c r="Q52" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R52" t="s">
-        <v>443</v>
+        <v>290</v>
       </c>
       <c r="T52" t="s">
-        <v>504</v>
+        <v>352</v>
       </c>
     </row>
     <row r="53" spans="1:20">
@@ -4712,44 +4260,44 @@
       <c r="E53" t="s">
         <v>228</v>
       </c>
-      <c r="F53" t="s">
-        <v>267</v>
-      </c>
-      <c r="H53" t="s">
-        <v>321</v>
-      </c>
-      <c r="I53" t="s">
-        <v>375</v>
-      </c>
-      <c r="J53" t="s">
-        <v>378</v>
-      </c>
-      <c r="K53" t="s">
-        <v>379</v>
-      </c>
-      <c r="L53" t="s">
-        <v>379</v>
+      <c r="F53" s="2">
+        <v>41091</v>
+      </c>
+      <c r="H53">
+        <v>11.0279</v>
+      </c>
+      <c r="I53">
+        <v>49.3227</v>
+      </c>
+      <c r="J53">
+        <v>2</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>1</v>
       </c>
       <c r="M53" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N53" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O53" t="s">
-        <v>385</v>
+        <v>232</v>
       </c>
       <c r="P53" t="s">
-        <v>389</v>
+        <v>236</v>
       </c>
       <c r="Q53" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R53" t="s">
-        <v>444</v>
+        <v>291</v>
       </c>
       <c r="T53" t="s">
-        <v>505</v>
+        <v>353</v>
       </c>
     </row>
     <row r="54" spans="1:20">
@@ -4765,47 +4313,47 @@
       <c r="D54" t="s">
         <v>200</v>
       </c>
-      <c r="F54" t="s">
-        <v>268</v>
-      </c>
-      <c r="H54" t="s">
-        <v>322</v>
-      </c>
-      <c r="I54" t="s">
-        <v>376</v>
-      </c>
-      <c r="J54" t="s">
-        <v>378</v>
-      </c>
-      <c r="K54" t="s">
-        <v>378</v>
-      </c>
-      <c r="L54" t="s">
-        <v>379</v>
+      <c r="F54" s="2">
+        <v>41667</v>
+      </c>
+      <c r="H54">
+        <v>11.4645</v>
+      </c>
+      <c r="I54">
+        <v>48.1817</v>
+      </c>
+      <c r="J54">
+        <v>2</v>
+      </c>
+      <c r="K54">
+        <v>2</v>
+      </c>
+      <c r="L54">
+        <v>1</v>
       </c>
       <c r="M54" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N54" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O54" t="s">
-        <v>386</v>
+        <v>233</v>
       </c>
       <c r="P54" t="s">
-        <v>390</v>
+        <v>237</v>
       </c>
       <c r="Q54" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R54" t="s">
-        <v>445</v>
+        <v>292</v>
       </c>
       <c r="S54" t="s">
-        <v>455</v>
+        <v>303</v>
       </c>
       <c r="T54" t="s">
-        <v>506</v>
+        <v>354</v>
       </c>
     </row>
     <row r="55" spans="1:20">
@@ -4824,44 +4372,44 @@
       <c r="E55" t="s">
         <v>229</v>
       </c>
-      <c r="F55" t="s">
-        <v>269</v>
-      </c>
-      <c r="H55" t="s">
-        <v>323</v>
-      </c>
-      <c r="I55" t="s">
-        <v>377</v>
-      </c>
-      <c r="J55" t="s">
-        <v>378</v>
-      </c>
-      <c r="K55" t="s">
-        <v>380</v>
-      </c>
-      <c r="L55" t="s">
-        <v>379</v>
+      <c r="F55" s="2">
+        <v>42370</v>
+      </c>
+      <c r="H55">
+        <v>11.0572</v>
+      </c>
+      <c r="I55">
+        <v>47.4771</v>
+      </c>
+      <c r="J55">
+        <v>2</v>
+      </c>
+      <c r="K55">
+        <v>6</v>
+      </c>
+      <c r="L55">
+        <v>1</v>
       </c>
       <c r="M55" t="s">
-        <v>383</v>
+        <v>230</v>
       </c>
       <c r="N55" t="s">
-        <v>384</v>
+        <v>231</v>
       </c>
       <c r="O55" t="s">
-        <v>387</v>
+        <v>234</v>
       </c>
       <c r="P55" t="s">
-        <v>391</v>
+        <v>238</v>
       </c>
       <c r="Q55" t="s">
-        <v>393</v>
+        <v>240</v>
       </c>
       <c r="R55" t="s">
-        <v>446</v>
+        <v>293</v>
       </c>
       <c r="T55" t="s">
-        <v>507</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>